<commit_message>
Sequences from Barr Lab at Monash
</commit_message>
<xml_diff>
--- a/OtherReports/Monash.xlsx
+++ b/OtherReports/Monash.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t xml:space="preserve">crAssphage sequencing samples</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">QLD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-27.3755791 153.1491078</t>
   </si>
   <si>
     <t xml:space="preserve">PCR Gels</t>
@@ -129,7 +126,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -151,80 +148,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -268,7 +191,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,74 +200,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -355,7 +221,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,77 +245,29 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -465,19 +283,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,60 +307,40 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -567,7 +365,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -600,9 +398,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>266400</xdr:colOff>
+      <xdr:colOff>266040</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -615,8 +413,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4699440" y="3338280"/>
-          <a:ext cx="7364520" cy="3024000"/>
+          <a:off x="4809960" y="3338280"/>
+          <a:ext cx="7524000" cy="3023640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -637,9 +435,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>53640</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -652,8 +450,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="834120" y="3352680"/>
-          <a:ext cx="3843000" cy="3009240"/>
+          <a:off x="850680" y="3352680"/>
+          <a:ext cx="3936600" cy="3008880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -675,19 +473,19 @@
   </sheetPr>
   <dimension ref="B3:I49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.61"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,32 +636,35 @@
       <c r="G11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>23</v>
+      <c r="H11" s="0" t="n">
+        <v>-27.3755791</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>153.1491078</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="D34" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="E34" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" s="13" t="n">
         <v>6.1</v>
@@ -885,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" s="13" t="n">
         <v>9.9</v>
@@ -899,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" s="13" t="n">
         <v>12.4</v>
@@ -913,12 +714,12 @@
         <v>4</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" s="15" t="n">
+        <v>29</v>
+      </c>
+      <c r="D38" s="13" t="n">
         <v>30.1</v>
       </c>
-      <c r="E38" s="15" t="n">
+      <c r="E38" s="13" t="n">
         <v>1.34</v>
       </c>
     </row>
@@ -927,12 +728,12 @@
         <v>4</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="15" t="n">
+        <v>30</v>
+      </c>
+      <c r="D39" s="13" t="n">
         <v>9.5</v>
       </c>
-      <c r="E39" s="15" t="n">
+      <c r="E39" s="13" t="n">
         <v>1.41</v>
       </c>
     </row>
@@ -941,12 +742,12 @@
         <v>4</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="15" t="n">
+        <v>31</v>
+      </c>
+      <c r="D40" s="13" t="n">
         <v>9.2</v>
       </c>
-      <c r="E40" s="15" t="n">
+      <c r="E40" s="13" t="n">
         <v>1.48</v>
       </c>
     </row>
@@ -955,12 +756,12 @@
         <v>5</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="15" t="n">
+        <v>29</v>
+      </c>
+      <c r="D41" s="13" t="n">
         <v>6.6</v>
       </c>
-      <c r="E41" s="15" t="n">
+      <c r="E41" s="13" t="n">
         <v>1.45</v>
       </c>
     </row>
@@ -969,12 +770,12 @@
         <v>5</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="15" t="n">
+        <v>30</v>
+      </c>
+      <c r="D42" s="13" t="n">
         <v>7.2</v>
       </c>
-      <c r="E42" s="15" t="n">
+      <c r="E42" s="13" t="n">
         <v>2.11</v>
       </c>
     </row>
@@ -983,12 +784,12 @@
         <v>5</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="15" t="n">
+        <v>31</v>
+      </c>
+      <c r="D43" s="13" t="n">
         <v>13.2</v>
       </c>
-      <c r="E43" s="15" t="n">
+      <c r="E43" s="13" t="n">
         <v>1.85</v>
       </c>
     </row>
@@ -997,12 +798,12 @@
         <v>6</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="15" t="n">
+        <v>29</v>
+      </c>
+      <c r="D44" s="13" t="n">
         <v>6.8</v>
       </c>
-      <c r="E44" s="15" t="n">
+      <c r="E44" s="13" t="n">
         <v>1.45</v>
       </c>
     </row>
@@ -1011,12 +812,12 @@
         <v>6</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="15" t="n">
+        <v>30</v>
+      </c>
+      <c r="D45" s="13" t="n">
         <v>11.7</v>
       </c>
-      <c r="E45" s="15" t="n">
+      <c r="E45" s="13" t="n">
         <v>1.73</v>
       </c>
     </row>
@@ -1025,12 +826,12 @@
         <v>6</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="15" t="n">
+        <v>31</v>
+      </c>
+      <c r="D46" s="13" t="n">
         <v>11.5</v>
       </c>
-      <c r="E46" s="15" t="n">
+      <c r="E46" s="13" t="n">
         <v>1.67</v>
       </c>
     </row>
@@ -1039,12 +840,12 @@
         <v>8</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="15" t="n">
+        <v>29</v>
+      </c>
+      <c r="D47" s="13" t="n">
         <v>10.8</v>
       </c>
-      <c r="E47" s="15" t="n">
+      <c r="E47" s="13" t="n">
         <v>1.43</v>
       </c>
     </row>
@@ -1053,33 +854,33 @@
         <v>8</v>
       </c>
       <c r="C48" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="13" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="E48" s="13" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C49" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="15" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="E48" s="15" t="n">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" s="16" t="n">
+      <c r="D49" s="15" t="n">
         <v>6.1</v>
       </c>
-      <c r="E49" s="16" t="n">
+      <c r="E49" s="15" t="n">
         <v>1.21</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>